<commit_message>
add trashed items and payments
</commit_message>
<xml_diff>
--- a/public/dashboard/excel-sheets-examples/payments.xlsx
+++ b/public/dashboard/excel-sheets-examples/payments.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -62,10 +62,13 @@
     <t>Publisher Name</t>
   </si>
   <si>
-    <t>slip-image-name.png</t>
-  </si>
-  <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>slip-image-name-1.png</t>
+  </si>
+  <si>
+    <t>slip-image-name.-2png</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,7 +462,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -482,7 +485,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -506,7 +509,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H3" s="3"/>
     </row>

</xml_diff>